<commit_message>
Actualizar proyecto y arreglar punto de venta leer excel #time 2h
</commit_message>
<xml_diff>
--- a/SiExpress/Scripts/uploads/INFORME DE DISTRIBUCION DE CARGA.xlsx
+++ b/SiExpress/Scripts/uploads/INFORME DE DISTRIBUCION DE CARGA.xlsx
@@ -5,26 +5,26 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="8160"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="15480" windowHeight="9975"/>
   </bookViews>
   <sheets>
-    <sheet name="C34A2014" sheetId="12" r:id="rId1"/>
+    <sheet name="C3" sheetId="12" r:id="rId1"/>
     <sheet name="C35A2014" sheetId="15" r:id="rId2"/>
     <sheet name="CXXA2014" sheetId="16" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'C34A2014'!$A$1:$AE$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'C3'!$A$8:$AE$11</definedName>
   </definedNames>
   <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
   <si>
     <t>GRO.</t>
   </si>
@@ -35,6 +35,9 @@
     <t>CIA</t>
   </si>
   <si>
+    <t>INV</t>
+  </si>
+  <si>
     <t>BLT</t>
   </si>
   <si>
@@ -65,6 +68,9 @@
     <t>MI</t>
   </si>
   <si>
+    <t>FECHA DE ACTUALIZACION</t>
+  </si>
+  <si>
     <t>CONTADOR</t>
   </si>
   <si>
@@ -116,12 +122,30 @@
     <t>FECHA ENTREGA</t>
   </si>
   <si>
+    <t>X COB.MX DLLs</t>
+  </si>
+  <si>
     <t>NOTAS TEXTO</t>
   </si>
   <si>
+    <t>DOM</t>
+  </si>
+  <si>
+    <t>Cont.</t>
+  </si>
+  <si>
     <t>ACAPULCO</t>
   </si>
   <si>
+    <t xml:space="preserve">CONTENEDOR </t>
+  </si>
+  <si>
+    <t>N° FACTURA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FECHA DE </t>
+  </si>
+  <si>
     <t>ACTUALIZACION</t>
   </si>
   <si>
@@ -131,6 +155,9 @@
     <t>D.F.</t>
   </si>
   <si>
+    <t>CEDIS GUADALAJARA</t>
+  </si>
+  <si>
     <t>3-AZ</t>
   </si>
   <si>
@@ -155,6 +182,9 @@
     <t xml:space="preserve">FL.AMARILLA </t>
   </si>
   <si>
+    <t>FEDEX</t>
+  </si>
+  <si>
     <t xml:space="preserve">LETICIA HERNANDEZ BALBUENA </t>
   </si>
   <si>
@@ -173,42 +203,46 @@
     <t>780042098745/780042101355</t>
   </si>
   <si>
+    <t>5 DE AGOSTO DEL 2014</t>
+  </si>
+  <si>
     <t>PROVEEDOR</t>
   </si>
   <si>
-    <t xml:space="preserve">Cliente: ACOSTA CELIA, CIA:MI, </t>
-  </si>
-  <si>
-    <t>DOM (ID_TARIFA=3)</t>
-  </si>
-  <si>
-    <t>FEDEX  (referencia_fedex)</t>
-  </si>
-  <si>
-    <t>DOM (id_TARIFA=3)</t>
-  </si>
-  <si>
-    <t>OCURRE DOM (id_TARIFA=3)</t>
-  </si>
-  <si>
-    <t>X COB.MX DLLs (seguro)</t>
-  </si>
-  <si>
-    <t>Cont. (id_contenedor)</t>
-  </si>
-  <si>
-    <t>INV (referencia)</t>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>XX</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>A2014</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="172" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="173" formatCode="[$-80A]d&quot; de &quot;mmmm&quot; de &quot;yyyy;@"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,6 +282,18 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="8"/>
+      <name val="Castellar"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="8"/>
+      <name val="Chevara"/>
+    </font>
+    <font>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -277,17 +323,43 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
+      <i/>
+      <sz val="22"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="44"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -297,18 +369,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor indexed="55"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -338,6 +404,15 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -378,179 +453,174 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="173" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="15" fontId="6" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="8" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="16" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="15" fontId="6" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="8" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="9" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="6" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="8" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="8" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -577,13 +647,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:row>175</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>615</xdr:row>
+      <xdr:row>622</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -632,13 +702,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:row>175</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>615</xdr:row>
+      <xdr:row>622</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -687,13 +757,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>165</xdr:row>
+      <xdr:row>172</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>615</xdr:row>
+      <xdr:row>622</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -742,13 +812,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>165</xdr:row>
+      <xdr:row>172</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>615</xdr:row>
+      <xdr:row>622</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -797,13 +867,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:row>175</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>615</xdr:row>
+      <xdr:row>622</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -852,13 +922,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:row>175</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>615</xdr:row>
+      <xdr:row>622</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -907,13 +977,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:row>175</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>615</xdr:row>
+      <xdr:row>622</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -962,13 +1032,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:row>175</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>615</xdr:row>
+      <xdr:row>622</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1017,13 +1087,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:row>175</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>615</xdr:row>
+      <xdr:row>622</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1072,13 +1142,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:row>175</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>615</xdr:row>
+      <xdr:row>622</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1127,13 +1197,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:row>175</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>615</xdr:row>
+      <xdr:row>622</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1182,13 +1252,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:row>175</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>615</xdr:row>
+      <xdr:row>622</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1236,14 +1306,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>175</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>615</xdr:row>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>622</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1255,8 +1325,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3762375" y="33451800"/>
-          <a:ext cx="209550" cy="84991575"/>
+          <a:off x="4029075" y="33451800"/>
+          <a:ext cx="266700" cy="84991575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1291,14 +1361,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>175</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>615</xdr:row>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>622</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1310,8 +1380,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3762375" y="33451800"/>
-          <a:ext cx="209550" cy="84991575"/>
+          <a:off x="4029075" y="33451800"/>
+          <a:ext cx="266700" cy="84991575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1346,14 +1416,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>165</xdr:row>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>172</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>615</xdr:row>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>622</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1365,8 +1435,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3762375" y="32880300"/>
-          <a:ext cx="209550" cy="85563075"/>
+          <a:off x="4029075" y="32880300"/>
+          <a:ext cx="266700" cy="85563075"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1401,14 +1471,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>165</xdr:row>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>172</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>615</xdr:row>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>622</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1420,8 +1490,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3762375" y="32880300"/>
-          <a:ext cx="209550" cy="85563075"/>
+          <a:off x="4029075" y="32880300"/>
+          <a:ext cx="266700" cy="85563075"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1456,14 +1526,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>175</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>615</xdr:row>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>622</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1475,8 +1545,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3762375" y="33451800"/>
-          <a:ext cx="209550" cy="84991575"/>
+          <a:off x="4029075" y="33451800"/>
+          <a:ext cx="266700" cy="84991575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1511,14 +1581,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>175</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>615</xdr:row>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>622</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1530,8 +1600,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3762375" y="33451800"/>
-          <a:ext cx="209550" cy="84991575"/>
+          <a:off x="4029075" y="33451800"/>
+          <a:ext cx="266700" cy="84991575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1566,14 +1636,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>175</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>615</xdr:row>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>622</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1585,8 +1655,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3762375" y="33451800"/>
-          <a:ext cx="209550" cy="84991575"/>
+          <a:off x="4029075" y="33451800"/>
+          <a:ext cx="266700" cy="84991575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1621,14 +1691,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>175</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>615</xdr:row>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>622</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1640,8 +1710,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3762375" y="33451800"/>
-          <a:ext cx="209550" cy="84991575"/>
+          <a:off x="4029075" y="33451800"/>
+          <a:ext cx="266700" cy="84991575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1676,14 +1746,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>175</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>615</xdr:row>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>622</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1695,8 +1765,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3762375" y="33451800"/>
-          <a:ext cx="209550" cy="84991575"/>
+          <a:off x="4029075" y="33451800"/>
+          <a:ext cx="266700" cy="84991575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1731,14 +1801,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>175</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>615</xdr:row>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>622</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1750,8 +1820,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3762375" y="33451800"/>
-          <a:ext cx="209550" cy="84991575"/>
+          <a:off x="4029075" y="33451800"/>
+          <a:ext cx="266700" cy="84991575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1786,14 +1856,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>175</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>615</xdr:row>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>622</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1805,8 +1875,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3762375" y="33451800"/>
-          <a:ext cx="209550" cy="84991575"/>
+          <a:off x="4029075" y="33451800"/>
+          <a:ext cx="266700" cy="84991575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1841,14 +1911,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>175</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>615</xdr:row>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>622</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1860,8 +1930,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3762375" y="33451800"/>
-          <a:ext cx="209550" cy="84991575"/>
+          <a:off x="4029075" y="33451800"/>
+          <a:ext cx="266700" cy="84991575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2181,478 +2251,613 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE16"/>
+  <dimension ref="A1:AE23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" style="16" customWidth="1"/>
-    <col min="5" max="5" width="15" style="16" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" style="16"/>
-    <col min="9" max="9" width="40.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="16"/>
-    <col min="14" max="14" width="15.42578125" style="16" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="16"/>
-    <col min="16" max="16" width="11.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.5703125" style="16" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" style="16"/>
-    <col min="20" max="20" width="16.85546875" style="16" customWidth="1"/>
-    <col min="21" max="21" width="24.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.85546875" style="2" customWidth="1"/>
-    <col min="23" max="23" width="17.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19" style="16" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="9.140625" style="16"/>
-    <col min="28" max="28" width="10.42578125" style="16" customWidth="1"/>
-    <col min="29" max="29" width="9.140625" style="16"/>
-    <col min="30" max="30" width="18.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="9.140625" style="16"/>
+    <col min="1" max="1" width="3.7109375" style="54" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" style="54" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="54" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" style="54" customWidth="1"/>
+    <col min="5" max="8" width="11.42578125" style="54" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" style="54" customWidth="1"/>
+    <col min="10" max="10" width="28.42578125" style="54" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" style="54" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="11.42578125" style="54" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" style="54" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="54" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" style="54" customWidth="1"/>
+    <col min="17" max="17" width="11.42578125" style="54" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" style="54" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.42578125" style="54" customWidth="1"/>
+    <col min="20" max="20" width="16.85546875" style="54" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" style="54" customWidth="1"/>
+    <col min="22" max="22" width="14.85546875" style="10" customWidth="1"/>
+    <col min="23" max="23" width="17.85546875" style="54" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.42578125" style="60" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19" style="54" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="11.42578125" style="54" customWidth="1"/>
+    <col min="28" max="28" width="10.42578125" style="54" customWidth="1"/>
+    <col min="29" max="256" width="11.42578125" style="54" customWidth="1"/>
+    <col min="257" max="16384" width="9.140625" style="54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="3" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
+    <row r="1" spans="1:31" s="30" customFormat="1" ht="12">
+      <c r="D1" s="32"/>
+      <c r="E1" s="33"/>
+      <c r="T1" s="34"/>
+      <c r="V1" s="10"/>
+      <c r="X1" s="34"/>
+      <c r="Z1" s="35"/>
+      <c r="AA1" s="35"/>
+      <c r="AB1" s="35"/>
+      <c r="AC1" s="35"/>
+      <c r="AD1" s="35"/>
+    </row>
+    <row r="2" spans="1:31" s="30" customFormat="1" ht="12">
+      <c r="C2" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="32"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="37"/>
+      <c r="X2" s="38"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="39"/>
+      <c r="AA2" s="39"/>
+      <c r="AB2" s="35"/>
+      <c r="AC2" s="35"/>
+    </row>
+    <row r="3" spans="1:31" s="30" customFormat="1" ht="18.75">
+      <c r="C3" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="32"/>
+      <c r="E3" s="35"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="41"/>
+      <c r="R3" s="37"/>
+      <c r="S3" s="37"/>
+      <c r="T3" s="38"/>
+      <c r="U3" s="37"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="37"/>
+      <c r="X3" s="38"/>
+      <c r="Y3" s="37"/>
+      <c r="Z3" s="39"/>
+      <c r="AA3" s="39"/>
+      <c r="AB3" s="35"/>
+      <c r="AC3" s="42"/>
+      <c r="AD3" s="43"/>
+      <c r="AE3" s="43"/>
+    </row>
+    <row r="4" spans="1:31" s="30" customFormat="1" ht="12">
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="42"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43"/>
+      <c r="T4" s="34"/>
+      <c r="V4" s="10"/>
+      <c r="X4" s="34"/>
+      <c r="Z4" s="35"/>
+      <c r="AA4" s="35"/>
+      <c r="AB4" s="35"/>
+      <c r="AC4" s="42"/>
+      <c r="AD4" s="36"/>
+      <c r="AE4" s="36"/>
+    </row>
+    <row r="5" spans="1:31" s="30" customFormat="1" ht="28.5">
+      <c r="E5" s="42"/>
+      <c r="I5" s="67" t="s">
+        <v>43</v>
+      </c>
+      <c r="M5" s="43"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="43"/>
+      <c r="Q5" s="43"/>
+      <c r="T5" s="34"/>
+      <c r="V5" s="10"/>
+      <c r="X5" s="34"/>
+      <c r="Z5" s="35"/>
+      <c r="AA5" s="35"/>
+      <c r="AB5" s="35"/>
+      <c r="AC5" s="42"/>
+      <c r="AD5" s="43"/>
+      <c r="AE5" s="36"/>
+    </row>
+    <row r="6" spans="1:31" s="30" customFormat="1" ht="12">
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="42"/>
+      <c r="T6" s="34"/>
+      <c r="V6" s="10"/>
+      <c r="X6" s="34"/>
+      <c r="Z6" s="35"/>
+      <c r="AA6" s="35"/>
+      <c r="AB6" s="35"/>
+      <c r="AC6" s="42"/>
+      <c r="AD6" s="43"/>
+      <c r="AE6" s="36"/>
+    </row>
+    <row r="7" spans="1:31" s="30" customFormat="1" ht="12">
+      <c r="C7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="43"/>
+      <c r="P7" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="T7" s="34"/>
+      <c r="V7" s="10"/>
+      <c r="X7" s="34"/>
+      <c r="Z7" s="35"/>
+      <c r="AA7" s="35"/>
+      <c r="AB7" s="35"/>
+      <c r="AC7" s="46"/>
+      <c r="AD7" s="36"/>
+      <c r="AE7" s="36"/>
+    </row>
+    <row r="8" spans="1:31" s="12" customFormat="1" ht="12">
+      <c r="A8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="P8" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q8" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="R8" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="S8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="T8" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="U8" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="V8" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="W8" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="X8" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y8" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE8" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" s="30" customFormat="1" ht="15" customHeight="1">
+      <c r="A9" s="16">
+        <v>1</v>
+      </c>
+      <c r="B9" s="17">
+        <v>1</v>
+      </c>
+      <c r="C9" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="19" t="s">
+      <c r="F9" s="70" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="71">
         <v>1</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="H9" s="71">
+        <v>1</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="J9" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="K9" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="55">
+        <v>41846</v>
+      </c>
+      <c r="R9" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="S9" s="23"/>
+      <c r="T9" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="U9" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="V9" s="14">
+        <v>41845</v>
+      </c>
+      <c r="W9" s="23"/>
+      <c r="X9" s="49"/>
+      <c r="Y9" s="26"/>
+      <c r="Z9" s="61" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA9" s="20"/>
+      <c r="AB9" s="72">
+        <v>17</v>
+      </c>
+      <c r="AC9" s="66"/>
+      <c r="AD9" s="73"/>
+      <c r="AE9" s="74"/>
+    </row>
+    <row r="10" spans="1:31" s="30" customFormat="1" ht="15" customHeight="1">
+      <c r="A10" s="16">
+        <v>1</v>
+      </c>
+      <c r="B10" s="17">
+        <v>249</v>
+      </c>
+      <c r="C10" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="61" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="61">
+        <v>1</v>
+      </c>
+      <c r="H10" s="61">
+        <v>1</v>
+      </c>
+      <c r="I10" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="J10" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="55">
+        <v>41848</v>
+      </c>
+      <c r="R10" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="S10" s="23"/>
+      <c r="T10" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="U10" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="V10" s="14">
+        <v>41845</v>
+      </c>
+      <c r="W10" s="23"/>
+      <c r="X10" s="49"/>
+      <c r="Y10" s="26"/>
+      <c r="Z10" s="61" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA10" s="20"/>
+      <c r="AB10" s="72">
+        <v>28</v>
+      </c>
+      <c r="AC10" s="66"/>
+      <c r="AD10" s="75"/>
+      <c r="AE10" s="74"/>
+    </row>
+    <row r="11" spans="1:31" s="30" customFormat="1" ht="15" customHeight="1">
+      <c r="A11" s="16"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="55"/>
+      <c r="R11" s="25"/>
+      <c r="S11" s="23"/>
+      <c r="T11" s="49"/>
+      <c r="U11" s="23"/>
+      <c r="V11" s="14"/>
+      <c r="W11" s="23"/>
+      <c r="X11" s="49"/>
+      <c r="Y11" s="26"/>
+      <c r="Z11" s="20"/>
+      <c r="AA11" s="20"/>
+      <c r="AB11" s="65"/>
+      <c r="AC11" s="57"/>
+      <c r="AD11" s="58"/>
+      <c r="AE11" s="29"/>
+    </row>
+    <row r="12" spans="1:31" s="30" customFormat="1" ht="15" customHeight="1">
+      <c r="A12" s="16"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="25"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="49"/>
+      <c r="U12" s="29"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="56"/>
+      <c r="X12" s="49"/>
+      <c r="Y12" s="26"/>
+      <c r="Z12" s="20"/>
+      <c r="AA12" s="20"/>
+      <c r="AB12" s="20"/>
+      <c r="AC12" s="27"/>
+      <c r="AD12" s="28"/>
+      <c r="AE12" s="29"/>
+    </row>
+    <row r="13" spans="1:31" s="30" customFormat="1" ht="12">
+      <c r="A13" s="50">
+        <f>SUBTOTAL(9,A9:A12)</f>
         <v>2</v>
       </c>
-      <c r="F1" s="52" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="19" t="s">
+      <c r="B13" s="29"/>
+      <c r="C13" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="64" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" s="64" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="49" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="N1" s="64" t="s">
-        <v>20</v>
-      </c>
-      <c r="O1" s="68" t="s">
-        <v>21</v>
-      </c>
-      <c r="P1" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q1" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="R1" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="S1" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="T1" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="U1" s="49" t="s">
-        <v>25</v>
-      </c>
-      <c r="V1" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="W1" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="X1" s="71" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y1" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z1" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA1" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB1" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC1" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="AD1" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="AE1" s="19" t="s">
-        <v>30</v>
-      </c>
+      <c r="D13" s="50"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="50">
+        <f>SUBTOTAL(9,G9:G12)</f>
+        <v>2</v>
+      </c>
+      <c r="H13" s="50">
+        <f>SUBTOTAL(9,H9:H12)</f>
+        <v>2</v>
+      </c>
+      <c r="I13" s="50"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="50"/>
+      <c r="N13" s="50"/>
+      <c r="O13" s="50"/>
+      <c r="P13" s="50"/>
+      <c r="Q13" s="50"/>
+      <c r="R13" s="25"/>
+      <c r="S13" s="50"/>
+      <c r="T13" s="51"/>
+      <c r="U13" s="29"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="50"/>
+      <c r="X13" s="51"/>
+      <c r="Y13" s="50"/>
+      <c r="Z13" s="47"/>
+      <c r="AA13" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB13" s="47"/>
+      <c r="AC13" s="47"/>
+      <c r="AD13" s="52">
+        <f>SUM(AD9:AD12)</f>
+        <v>0</v>
+      </c>
+      <c r="AE13" s="53"/>
     </row>
-    <row r="2" spans="1:31" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="62">
-        <v>1</v>
-      </c>
-      <c r="B2" s="63">
-        <v>1</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="58" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="59" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="26">
-        <v>1</v>
-      </c>
-      <c r="H2" s="26">
-        <v>1</v>
-      </c>
-      <c r="I2" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="J2" s="65" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="65" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50">
-        <v>0</v>
-      </c>
-      <c r="N2" s="50" t="s">
-        <v>44</v>
-      </c>
-      <c r="O2" s="4"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="32">
-        <v>41846</v>
-      </c>
-      <c r="R2" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="S2" s="31"/>
-      <c r="T2" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="U2" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="V2" s="37">
-        <v>41845</v>
-      </c>
-      <c r="W2" s="39"/>
-      <c r="X2" s="40"/>
-      <c r="Y2" s="72"/>
-      <c r="Z2" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA2" s="28"/>
-      <c r="AB2" s="43">
-        <v>17</v>
-      </c>
-      <c r="AC2" s="46"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="57"/>
-    </row>
-    <row r="3" spans="1:31" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="62">
-        <v>1</v>
-      </c>
-      <c r="B3" s="63">
-        <v>249</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="58" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="60" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="24">
-        <v>1</v>
-      </c>
-      <c r="H3" s="24">
-        <v>1</v>
-      </c>
-      <c r="I3" s="50" t="s">
-        <v>46</v>
-      </c>
-      <c r="J3" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="65" t="s">
-        <v>0</v>
-      </c>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50">
-        <v>0</v>
-      </c>
-      <c r="N3" s="50" t="s">
-        <v>47</v>
-      </c>
-      <c r="O3" s="4"/>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="32">
-        <v>41848</v>
-      </c>
-      <c r="R3" s="69" t="s">
-        <v>52</v>
-      </c>
-      <c r="S3" s="50"/>
-      <c r="T3" s="70" t="s">
-        <v>48</v>
-      </c>
-      <c r="U3" s="50" t="s">
-        <v>53</v>
-      </c>
-      <c r="V3" s="37">
-        <v>41845</v>
-      </c>
-      <c r="W3" s="39"/>
-      <c r="X3" s="40"/>
-      <c r="Y3" s="72"/>
-      <c r="Z3" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA3" s="28"/>
-      <c r="AB3" s="43">
-        <v>28</v>
-      </c>
-      <c r="AC3" s="46"/>
-      <c r="AD3" s="54"/>
-      <c r="AE3" s="57"/>
-    </row>
-    <row r="4" spans="1:31" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="62"/>
-      <c r="B4" s="63"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="66"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="50"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="31"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="34"/>
-      <c r="S4" s="31"/>
-      <c r="T4" s="36"/>
-      <c r="U4" s="50" t="s">
-        <v>54</v>
-      </c>
-      <c r="V4" s="37"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="6"/>
-      <c r="Z4" s="28"/>
-      <c r="AA4" s="28"/>
-      <c r="AB4" s="44"/>
-      <c r="AC4" s="47"/>
-      <c r="AD4" s="55"/>
-      <c r="AE4" s="38"/>
-    </row>
-    <row r="5" spans="1:31" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="62"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="67"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="50"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="31"/>
-      <c r="R5" s="34"/>
-      <c r="S5" s="31"/>
-      <c r="T5" s="36"/>
-      <c r="U5" s="51"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="17"/>
-      <c r="X5" s="11"/>
-      <c r="Y5" s="6"/>
-      <c r="Z5" s="28"/>
-      <c r="AA5" s="28"/>
-      <c r="AB5" s="28"/>
-      <c r="AC5" s="48"/>
-      <c r="AD5" s="56"/>
-      <c r="AE5" s="38"/>
-    </row>
-    <row r="6" spans="1:31" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A6" s="12">
-        <f>SUBTOTAL(9,A2:A5)</f>
-        <v>2</v>
-      </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12">
-        <f>SUBTOTAL(9,G2:G5)</f>
-        <v>2</v>
-      </c>
-      <c r="H6" s="12">
-        <f>SUBTOTAL(9,H2:H5)</f>
-        <v>2</v>
-      </c>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="12"/>
-      <c r="X6" s="13"/>
-      <c r="Y6" s="12"/>
-      <c r="Z6" s="9"/>
-      <c r="AA6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB6" s="9"/>
-      <c r="AC6" s="9"/>
-      <c r="AD6" s="14">
-        <f>SUM(AD2:AD5)</f>
-        <v>0</v>
-      </c>
-      <c r="AE6" s="15"/>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="R7"/>
-      <c r="S7"/>
-      <c r="T7"/>
-      <c r="U7"/>
-      <c r="V7" s="3"/>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="R8"/>
-      <c r="S8"/>
-      <c r="T8"/>
-      <c r="U8"/>
-      <c r="V8" s="3"/>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="R9"/>
-      <c r="S9"/>
-      <c r="T9"/>
-      <c r="U9"/>
-      <c r="V9" s="3"/>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="C10" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="R10"/>
-      <c r="S10"/>
-      <c r="T10"/>
-      <c r="U10"/>
-      <c r="V10" s="3"/>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="R11"/>
-      <c r="S11"/>
-      <c r="T11"/>
-      <c r="U11"/>
-      <c r="V11" s="3"/>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="R12"/>
-      <c r="S12"/>
-      <c r="T12"/>
-      <c r="U12"/>
-      <c r="V12" s="3"/>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="R13"/>
-      <c r="S13"/>
-      <c r="T13"/>
-      <c r="U13"/>
-      <c r="V13" s="3"/>
-    </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31">
       <c r="R14"/>
       <c r="S14"/>
       <c r="T14"/>
       <c r="U14"/>
-      <c r="V14" s="3"/>
+      <c r="V14" s="12"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31">
       <c r="R15"/>
       <c r="S15"/>
       <c r="T15"/>
       <c r="U15"/>
-      <c r="V15" s="3"/>
+      <c r="V15" s="12"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31">
       <c r="R16"/>
       <c r="S16"/>
       <c r="T16"/>
       <c r="U16"/>
+      <c r="V16" s="12"/>
+    </row>
+    <row r="17" spans="18:22">
+      <c r="R17"/>
+      <c r="S17"/>
+      <c r="T17"/>
+      <c r="U17"/>
+      <c r="V17" s="12"/>
+    </row>
+    <row r="18" spans="18:22">
+      <c r="R18"/>
+      <c r="S18"/>
+      <c r="T18"/>
+      <c r="U18"/>
+      <c r="V18" s="12"/>
+    </row>
+    <row r="19" spans="18:22">
+      <c r="R19"/>
+      <c r="S19"/>
+      <c r="T19"/>
+      <c r="U19"/>
+      <c r="V19" s="12"/>
+    </row>
+    <row r="20" spans="18:22">
+      <c r="R20"/>
+      <c r="S20"/>
+      <c r="T20"/>
+      <c r="U20"/>
+      <c r="V20" s="12"/>
+    </row>
+    <row r="21" spans="18:22">
+      <c r="R21"/>
+      <c r="S21"/>
+      <c r="T21"/>
+      <c r="U21"/>
+      <c r="V21" s="12"/>
+    </row>
+    <row r="22" spans="18:22">
+      <c r="R22"/>
+      <c r="S22"/>
+      <c r="T22"/>
+      <c r="U22"/>
+      <c r="V22" s="12"/>
+    </row>
+    <row r="23" spans="18:22">
+      <c r="R23"/>
+      <c r="S23"/>
+      <c r="T23"/>
+      <c r="U23"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <drawing r:id="rId1"/>
@@ -2665,9 +2870,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -2678,9 +2883,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>